<commit_message>
Agregar info de modelo a excel
</commit_message>
<xml_diff>
--- a/Resultados_Optimización.xlsx
+++ b/Resultados_Optimización.xlsx
@@ -7,11 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Procesos Activados" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Procesos en Operación" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Rebalses" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Total Contaminantes Z" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Concentraciones" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Información Modelo" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Procesos Activados" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Procesos en Operación" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Rebalses" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Total Contaminantes Z" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Concentraciones" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,6 +430,85 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Valor objetivo</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GAP</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Tiempo de resolución (segundos)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cantidad de variables</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cantidad de restricciones</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Cantidad de variables binarias</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Cantidad de variables continuas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12590099146.80001</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.105000019073486</v>
+      </c>
+      <c r="D2" t="n">
+        <v>15695</v>
+      </c>
+      <c r="E2" t="n">
+        <v>23096</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4380</v>
+      </c>
+      <c r="G2" t="n">
+        <v>11315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -478,7 +558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3429,7 +3509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6783,77 +6863,6 @@
         <is>
           <t>Proceso</t>
         </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Contaminante</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Total_Z</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>3076725954.240003</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2216138946.480002</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2969627806.080002</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>141557220.0000001</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>4186049219.999999</v>
       </c>
     </row>
   </sheetData>
@@ -6883,6 +6892,77 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Total_Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3076725954.240003</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2216138946.480002</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2969627806.080002</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>141557220.0000001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4186049219.999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contaminante</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Concentración en salida</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Agregar archivos de debug
</commit_message>
<xml_diff>
--- a/Resultados_Optimización.xlsx
+++ b/Resultados_Optimización.xlsx
@@ -477,13 +477,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>12590099146.80001</v>
+        <v>12588076900.80002</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>2.105000019073486</v>
+        <v>2.11</v>
       </c>
       <c r="D2" t="n">
         <v>15695</v>
@@ -6925,7 +6925,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>141557220.0000001</v>
+        <v>139534974</v>
       </c>
     </row>
     <row r="6">
@@ -6972,7 +6972,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1141080000000001</v>
+        <v>0.114108</v>
       </c>
     </row>
     <row r="3">
@@ -6980,7 +6980,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.08219100000000007</v>
+        <v>0.082191</v>
       </c>
     </row>
     <row r="4">
@@ -6988,7 +6988,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1101360000000001</v>
+        <v>0.110136</v>
       </c>
     </row>
     <row r="5">
@@ -6996,7 +6996,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.005250000000000005</v>
+        <v>0.005175</v>
       </c>
     </row>
     <row r="6">
@@ -7004,7 +7004,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1552499999999999</v>
+        <v>0.15525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>